<commit_message>
DFM changes to bebl_v2 based on seeed feedback
</commit_message>
<xml_diff>
--- a/kicad/PCB Technology Requirement Format V1 for bebl_v2.xlsx
+++ b/kicad/PCB Technology Requirement Format V1 for bebl_v2.xlsx
@@ -15,11 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
-  <si>
-    <r>
-      <t>                         深圳矽递科技有限公司
-                          </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <r>
+      <t>深圳矽递科技有限公司</t>
     </r>
     <r>
       <rPr>
@@ -29,7 +28,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Seeed Technology Limited</t>
+      <t>Seeed Technology Inc.</t>
     </r>
   </si>
   <si>
@@ -37,9 +36,6 @@
   </si>
   <si>
     <t>PCB Name &amp; Version</t>
-  </si>
-  <si>
-    <t>bebl_v2</t>
   </si>
   <si>
     <r>
@@ -53,21 +49,22 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>板材：</t>
     </r>
   </si>
   <si>
     <r>
-      <t>  
-    (Rigid)FR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+      <t>(Rigid)FR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>－</t>
     </r>
@@ -79,12 +76,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>4
-</t>
-    </r>
-  </si>
-  <si>
-    <t>                     Flex</t>
+      <t>4</t>
+    </r>
   </si>
   <si>
     <r>
@@ -98,15 +91,16 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>大小：</t>
     </r>
   </si>
   <si>
-    <t>    cm        mm        inch</t>
-  </si>
-  <si>
-    <t>(                      ) × (                       )</t>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>(    80         ) × (    24      )</t>
   </si>
   <si>
     <r>
@@ -120,12 +114,10 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>层数：</t>
     </r>
-  </si>
-  <si>
-    <t>other:(           )</t>
   </si>
   <si>
     <r>
@@ -139,257 +131,153 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>厚度：</t>
     </r>
   </si>
   <si>
-    <t>      0.8mm</t>
-  </si>
-  <si>
-    <t>        1.2mm</t>
-  </si>
-  <si>
-    <t>    1mm </t>
-  </si>
-  <si>
-    <t>        1.6mm</t>
-  </si>
-  <si>
-    <r>
-      <t>Copper Weight
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+    <t>1.6mm</t>
+  </si>
+  <si>
+    <r>
+      <t>Copper Weight</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>铜厚：</t>
     </r>
   </si>
   <si>
-    <t> 1oz</t>
-  </si>
-  <si>
-    <t> 2oz</t>
-  </si>
-  <si>
-    <t>other:(            )</t>
-  </si>
-  <si>
-    <r>
-      <t>PCB Colour
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+    <t>1oz</t>
+  </si>
+  <si>
+    <r>
+      <t>PCB Colour</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>阻焊颜色：</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Green
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-      </rPr>
-      <t>绿色</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>White
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+      <t>White</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>白色</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Black
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+      <t>Silkscreen</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>字符颜色：</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Black</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>黑色</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Red
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-      </rPr>
-      <t>红色</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Blue
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-      </rPr>
-      <t>蓝色</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Silkscreen
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-      </rPr>
-      <t>字符颜色：</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Pads Finished
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+      <t>Pads Finished</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>焊盘喷镀：</t>
     </r>
   </si>
   <si>
     <r>
-      <t> (Hasl-lead free)   
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+      <t>(Hasl-lead free)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>无铅喷锡</t>
     </r>
   </si>
   <si>
     <r>
-      <t>(Hasl)    
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-      </rPr>
-      <t>含铅喷锡</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>(ENIG)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-      </rPr>
-      <t>沉镍金</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Via solder mask
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+      <t>Via solder mask</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>阻焊覆盖：</t>
     </r>
   </si>
   <si>
     <r>
-      <t>solder mask  cover
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-      </rPr>
-      <t>过孔盖油</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>solder mask  opening 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+      <t>solder mask  opening</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>过孔开窗</t>
     </r>
@@ -397,61 +285,72 @@
   <si>
     <r>
       <t>Minimum trace/space
-(mm)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+(mm)</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>最小线宽</t>
     </r>
   </si>
   <si>
+    <t>0.178mm</t>
+  </si>
+  <si>
     <r>
       <t>Minimum hole size
-(mm)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+(mm)</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>最小孔径</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>Special requirements
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
+    <t>0.508mm</t>
+  </si>
+  <si>
+    <r>
+      <t>Special requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>特殊工艺：</t>
     </r>
   </si>
   <si>
-    <t> Yes</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>(Put requirements here)</t>
   </si>
   <si>
     <t>Comment:</t>
+  </si>
+  <si>
+    <t>PCB is in two parts
+80 x 24 mm
+74 x 11 mm</t>
   </si>
 </sst>
 </file>
@@ -497,6 +396,7 @@
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -528,6 +428,7 @@
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -720,8 +621,8 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -777,7 +678,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -857,15 +758,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>65160</xdr:colOff>
+      <xdr:colOff>119160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>697680</xdr:colOff>
+      <xdr:colOff>750960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>476280</xdr:rowOff>
+      <xdr:rowOff>457560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -878,8 +779,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="65160" y="38520"/>
-          <a:ext cx="632520" cy="437760"/>
+          <a:off x="119160" y="20520"/>
+          <a:ext cx="631800" cy="437040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -902,18 +803,18 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2388663967611"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.0526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.7692307692308"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8663967611336"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.9797570850202"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.5263157894737"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.25506072874494"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.6234817813765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3724696356275"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2550607287449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.3765182186235"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3724696356275"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.1255060728745"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -944,9 +845,7 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="0"/>
@@ -956,29 +855,27 @@
     </row>
     <row r="4" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="9"/>
       <c r="E4" s="0"/>
       <c r="F4" s="10"/>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>9</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="0"/>
@@ -986,19 +883,15 @@
       <c r="G5" s="0"/>
       <c r="H5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
@@ -1006,17 +899,11 @@
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -1024,11 +911,9 @@
     </row>
     <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
-      <c r="B8" s="15" t="s">
-        <v>15</v>
-      </c>
+      <c r="B8" s="15"/>
       <c r="C8" s="14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="16"/>
@@ -1038,17 +923,13 @@
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>20</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -1056,17 +937,13 @@
     </row>
     <row r="10" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>22</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>24</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D10" s="19"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -1074,15 +951,9 @@
     </row>
     <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
-      <c r="B11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -1090,71 +961,67 @@
     </row>
     <row r="12" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>23</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B12" s="17"/>
       <c r="C12" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>20</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>31</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
     </row>
     <row r="14" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>33</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B14" s="17"/>
       <c r="C14" s="18" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="C15" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="21"/>
+        <v>23</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="25"/>
+        <v>28</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
     </row>

</xml_diff>